<commit_message>
update verify list column
</commit_message>
<xml_diff>
--- a/exam/src/main/webapp/exam/WEB-INF/template/excelExport.xlsx
+++ b/exam/src/main/webapp/exam/WEB-INF/template/excelExport.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14128"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\EBT\work\exam\src\main\webapp\exam\WEB-INF\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
@@ -16,229 +11,21 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$R$2</definedName>
+  </definedNames>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>${applyUsers.applyUserName}</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>${applyUsers.applyUserHomeTown}</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>${applyUsers.idCardNo}</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>姓名</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>身份</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>证</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>号</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>籍</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>贯</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>政治面貌</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>报</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>考部</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>门</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>岗</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>类别</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>岗</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>编</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>号</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>审</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>核状</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>态</t>
-    </r>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
@@ -376,6 +163,18 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>性别</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>专业</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>学历</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>${applyUsers.aplyUserPolitical == "1" ? "</t>
     </r>
@@ -422,7 +221,16 @@
         <family val="3"/>
         <charset val="128"/>
       </rPr>
-      <t>群众</t>
+      <t>群</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>众</t>
     </r>
     <r>
       <rPr>
@@ -437,69 +245,161 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="FangSong"/>
+      <t>${applyUsers.user.sex == "1" ? "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>报</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>名人</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="FangSong"/>
+      <t>男</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>员</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>信息一</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>览</t>
-    </r>
+      <t>女</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>"}</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.user.graduateSchool}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.user.major}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.user.degree}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.user.birthdayYear}/${applyUsers.user.birthdayMonth}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.user.graduateYear}/${applyUsers.user.graduateMonth}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算机程度</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>联系电话</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.user.computerSkill}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.user.languageSkill}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.user.telephone}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.user.height}cm</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>报名人员信息一览</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>政治面貌</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>出生年月</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>毕业院校</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>毕业时间</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>外语程度</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>身高</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.applyUserName}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>身份证号</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>籍贯</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>报考部门</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>岗位类别</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>岗位编号</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>审核状态</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -516,20 +416,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <name val="FangSong"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="FangSong"/>
       <family val="3"/>
@@ -540,6 +426,34 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -589,25 +503,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -665,7 +581,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
@@ -700,7 +616,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
@@ -877,100 +793,183 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="32" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="L2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:18" ht="12.75" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="R4" s="5" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:R2"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -979,12 +978,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -993,12 +992,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
format src; update room and seat; update admission print;...
</commit_message>
<xml_diff>
--- a/exam/src/main/webapp/exam/WEB-INF/template/excelExport.xlsx
+++ b/exam/src/main/webapp/exam/WEB-INF/template/excelExport.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\EBT\work\exam\src\main\webapp\exam\WEB-INF\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
@@ -17,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$V$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$Z$2</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>${applyUsers.applyUserHomeTown}</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -561,13 +556,142 @@
   </si>
   <si>
     <t>${applyUsers.user.socialRel}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>考</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>场</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>座位号</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>准考</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>证</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>${applyUsers.room.code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.seat.code}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>${applyUsers.admission.code}</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>准考证打印状态</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>${applyUsers.admission != null ? applyUsers.admission.printFlg ? "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>否</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>":""}</t>
+    </r>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -609,7 +733,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="ＭＳ ゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -617,14 +741,14 @@
     <font>
       <b/>
       <sz val="10"/>
-      <name val="ＭＳ ゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="ＭＳ ゴシック"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -700,7 +824,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -970,17 +1094,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -1005,15 +1131,15 @@
     <col min="19" max="19" width="15.28515625" customWidth="1"/>
     <col min="20" max="20" width="13.85546875" customWidth="1"/>
     <col min="21" max="21" width="8.85546875" customWidth="1"/>
-    <col min="22" max="22" width="11.140625" customWidth="1"/>
+    <col min="22" max="26" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:26">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:26">
       <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
@@ -1080,8 +1206,20 @@
       <c r="V2" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="W2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" ht="12.75" customHeight="1">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
@@ -1148,8 +1286,20 @@
       <c r="V3" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="W3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:26">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1176,9 +1326,21 @@
       <c r="V4" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="W4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:V2"/>
+  <autoFilter ref="A2:Z2"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1187,7 +1349,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1201,7 +1363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>